<commit_message>
adding hz light test validation with light simulation software
</commit_message>
<xml_diff>
--- a/prj/fermentabot/FMT201/Fermentabot Sample Data 12-21-18.xlsx
+++ b/prj/fermentabot/FMT201/Fermentabot Sample Data 12-21-18.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Open AG\Documents\GitHub\openag-mechanical\prj\fermentabot\FMT201\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E8D0E0A8-A9A4-44F9-8618-135BEB30A704}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{B3A0BF5A-D95C-462D-9C0F-5E7C3099ADA0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24310" windowHeight="15160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24310" windowHeight="15160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="tmp_2016_us" sheetId="1" r:id="rId1"/>
+    <sheet name="Extended Test" sheetId="1" r:id="rId1"/>
+    <sheet name="Start-up Test" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
   <si>
     <t>Date</t>
   </si>
@@ -691,7 +692,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>tmp_2016_us!$C$5:$C$342</c:f>
+              <c:f>'Extended Test'!$C$5:$C$342</c:f>
               <c:numCache>
                 <c:formatCode>h:mm:ss</c:formatCode>
                 <c:ptCount val="338"/>
@@ -1714,7 +1715,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>tmp_2016_us!$D$5:$D$342</c:f>
+              <c:f>'Extended Test'!$D$5:$D$342</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="338"/>
@@ -2762,7 +2763,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>tmp_2016_us!$C$5:$C$342</c:f>
+              <c:f>'Extended Test'!$C$5:$C$342</c:f>
               <c:numCache>
                 <c:formatCode>h:mm:ss</c:formatCode>
                 <c:ptCount val="338"/>
@@ -3785,7 +3786,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>tmp_2016_us!$G$5:$G$342</c:f>
+              <c:f>'Extended Test'!$G$5:$G$342</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="338"/>
@@ -5259,7 +5260,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>tmp_2016_us!$C$5:$C$342</c:f>
+              <c:f>'Extended Test'!$C$5:$C$342</c:f>
               <c:numCache>
                 <c:formatCode>h:mm:ss</c:formatCode>
                 <c:ptCount val="338"/>
@@ -6282,7 +6283,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>tmp_2016_us!$E$5:$E$342</c:f>
+              <c:f>'Extended Test'!$E$5:$E$342</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="338"/>
@@ -7330,7 +7331,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>tmp_2016_us!$C$5:$C$342</c:f>
+              <c:f>'Extended Test'!$C$5:$C$342</c:f>
               <c:numCache>
                 <c:formatCode>h:mm:ss</c:formatCode>
                 <c:ptCount val="338"/>
@@ -8353,7 +8354,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>tmp_2016_us!$H$5:$H$341</c:f>
+              <c:f>'Extended Test'!$H$5:$H$341</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="337"/>
@@ -9721,6 +9722,1927 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1"/>
+              <a:t>Temperature vs Time </a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="6.828126825393116E-2"/>
+          <c:y val="7.1879844961240308E-2"/>
+          <c:w val="0.89628110469870792"/>
+          <c:h val="0.84206723432826713"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Top Tray</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Start-up Test'!$B$5:$B$342</c:f>
+              <c:numCache>
+                <c:formatCode>h:mm:ss</c:formatCode>
+                <c:ptCount val="338"/>
+                <c:pt idx="0">
+                  <c:v>0.68078703703703702</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.68113425925925919</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.68148148148148147</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.68182870370370363</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.68217592592592602</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.68252314814814818</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.68287037037037035</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.68321759259259263</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.68356481481481479</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.68391203703703696</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.68425925925925923</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.68460648148148151</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.68495370370370379</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.68530092592592595</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.68564814814814812</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.68599537037037039</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.68634259259259256</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.68668981481481473</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.687037037037037</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.68738425925925928</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.68773148148148155</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.68807870370370372</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.68842592592592589</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.68877314814814816</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.68912037037037033</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.68946759259259249</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.68981481481481488</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.69016203703703705</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.69050925925925932</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.69085648148148149</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.69120370370370365</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.69155092592592593</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.6918981481481481</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.69224537037037026</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.69259259259259265</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.69293981481481481</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.69328703703703709</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.69363425925925926</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.69398148148148142</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.6943287037037037</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.69467592592592586</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.69502314814814825</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.69537037037037042</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.69571759259259258</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.69606481481481486</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.69641203703703702</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.69675925925925919</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.69710648148148147</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.69745370370370363</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.69780092592592602</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.69814814814814818</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.69849537037037035</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.69884259259259263</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.69918981481481479</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Start-up Test'!$C$5:$C$342</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="338"/>
+                <c:pt idx="0">
+                  <c:v>28.869199999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28.5045</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>28.2042</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>28.011199999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>27.9147</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>27.9254</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>27.989699999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>28.107700000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>28.2364</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>28.397300000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>28.579599999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>28.7727</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>28.976400000000002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>29.180199999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>29.3947</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>29.598500000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>29.802299999999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>30.006</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>30.209800000000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>30.381399999999999</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>30.499400000000001</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>30.6067</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>30.756799999999998</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>30.907</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>31.046399999999998</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>31.121500000000001</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>31.153600000000001</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>31.218</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>31.314499999999999</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>31.411000000000001</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>31.443200000000001</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>31.464700000000001</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>31.529</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>31.625499999999999</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>31.689900000000002</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>31.689900000000002</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>31.689900000000002</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>31.722100000000001</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>31.7971</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>31.861499999999999</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>31.872199999999999</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>31.84</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>31.84</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>31.904399999999999</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>31.925799999999999</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>31.936599999999999</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>31.925799999999999</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>31.925799999999999</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>31.936599999999999</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>31.936599999999999</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>31.936599999999999</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>31.936599999999999</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>31.957999999999998</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>32.000900000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-05C4-4FEE-99C1-EB972168CC1D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Middle Tray</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="7030A0"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Start-up Test'!$B$5:$B$342</c:f>
+              <c:numCache>
+                <c:formatCode>h:mm:ss</c:formatCode>
+                <c:ptCount val="338"/>
+                <c:pt idx="0">
+                  <c:v>0.68078703703703702</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.68113425925925919</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.68148148148148147</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.68182870370370363</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.68217592592592602</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.68252314814814818</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.68287037037037035</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.68321759259259263</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.68356481481481479</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.68391203703703696</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.68425925925925923</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.68460648148148151</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.68495370370370379</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.68530092592592595</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.68564814814814812</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.68599537037037039</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.68634259259259256</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.68668981481481473</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.687037037037037</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.68738425925925928</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.68773148148148155</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.68807870370370372</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.68842592592592589</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.68877314814814816</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.68912037037037033</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.68946759259259249</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.68981481481481488</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.69016203703703705</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.69050925925925932</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.69085648148148149</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.69120370370370365</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.69155092592592593</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.6918981481481481</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.69224537037037026</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.69259259259259265</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.69293981481481481</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.69328703703703709</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.69363425925925926</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.69398148148148142</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.6943287037037037</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.69467592592592586</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.69502314814814825</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.69537037037037042</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.69571759259259258</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.69606481481481486</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.69641203703703702</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.69675925925925919</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.69710648148148147</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.69745370370370363</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.69780092592592602</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.69814814814814818</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.69849537037037035</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.69884259259259263</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.69918981481481479</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Start-up Test'!#REF!</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-05C4-4FEE-99C1-EB972168CC1D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="717779032"/>
+        <c:axId val="717780672"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="717779032"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="0.70100000000000007"/>
+          <c:min val="0.68000000000000016"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Time</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="h:mm:ss" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="717780672"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="6.9444440000000019E-3"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="717780672"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Temperature (°C)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="717779032"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1"/>
+              <a:t>Humidity vs Time </a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="6.828126825393116E-2"/>
+          <c:y val="7.1879844961240308E-2"/>
+          <c:w val="0.89628110469870792"/>
+          <c:h val="0.84206723432826713"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Top Tray</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Start-up Test'!$B$5:$B$342</c:f>
+              <c:numCache>
+                <c:formatCode>h:mm:ss</c:formatCode>
+                <c:ptCount val="338"/>
+                <c:pt idx="0">
+                  <c:v>0.68078703703703702</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.68113425925925919</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.68148148148148147</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.68182870370370363</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.68217592592592602</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.68252314814814818</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.68287037037037035</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.68321759259259263</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.68356481481481479</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.68391203703703696</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.68425925925925923</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.68460648148148151</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.68495370370370379</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.68530092592592595</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.68564814814814812</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.68599537037037039</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.68634259259259256</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.68668981481481473</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.687037037037037</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.68738425925925928</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.68773148148148155</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.68807870370370372</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.68842592592592589</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.68877314814814816</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.68912037037037033</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.68946759259259249</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.68981481481481488</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.69016203703703705</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.69050925925925932</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.69085648148148149</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.69120370370370365</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.69155092592592593</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.6918981481481481</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.69224537037037026</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.69259259259259265</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.69293981481481481</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.69328703703703709</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.69363425925925926</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.69398148148148142</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.6943287037037037</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.69467592592592586</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.69502314814814825</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.69537037037037042</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.69571759259259258</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.69606481481481486</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.69641203703703702</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.69675925925925919</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.69710648148148147</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.69745370370370363</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.69780092592592602</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.69814814814814818</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.69849537037037035</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.69884259259259263</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.69918981481481479</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Start-up Test'!$D$5:$D$342</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="338"/>
+                <c:pt idx="0">
+                  <c:v>42.961599999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>47.150199999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>51.865099999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>55.7714</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>56.542000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>55.061900000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>56.953899999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>60.356699999999996</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>60.4482</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>62.607300000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>62.111400000000003</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>62.706499999999998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>63.683100000000003</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>64.468900000000005</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>64.644400000000005</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>66.048199999999994</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>65.666700000000006</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>66.681399999999996</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>67.375699999999995</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>67.940299999999993</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>68.199700000000007</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>68.794799999999995</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>70.244399999999999</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>72.563699999999997</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>73.67</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>74.326099999999997</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>74.242199999999997</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>74.974599999999995</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>75.806200000000004</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>76.698800000000006</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>77.179500000000004</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>77.744</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>79.979500000000002</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>80.299899999999994</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>81.177300000000002</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>81.375600000000006</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>82.092799999999997</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>82.672600000000003</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>84.602900000000005</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>84.602900000000005</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>85.152199999999993</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>85.793099999999995</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>86.8917</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>87.593599999999995</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>87.998000000000005</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>88.173400000000001</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>88.257400000000004</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>88.898200000000003</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>89.554400000000001</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>89.874799999999993</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>89.523799999999994</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>89.813800000000001</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>90.080799999999996</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>90.485100000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F8FA-4640-A230-8DCCF7D0B504}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Middle Tray</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="7030A0"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Start-up Test'!$B$5:$B$342</c:f>
+              <c:numCache>
+                <c:formatCode>h:mm:ss</c:formatCode>
+                <c:ptCount val="338"/>
+                <c:pt idx="0">
+                  <c:v>0.68078703703703702</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.68113425925925919</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.68148148148148147</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.68182870370370363</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.68217592592592602</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.68252314814814818</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.68287037037037035</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.68321759259259263</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.68356481481481479</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.68391203703703696</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.68425925925925923</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.68460648148148151</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.68495370370370379</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.68530092592592595</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.68564814814814812</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.68599537037037039</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.68634259259259256</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.68668981481481473</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.687037037037037</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.68738425925925928</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.68773148148148155</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.68807870370370372</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.68842592592592589</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.68877314814814816</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.68912037037037033</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.68946759259259249</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.68981481481481488</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.69016203703703705</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.69050925925925932</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.69085648148148149</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.69120370370370365</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.69155092592592593</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.6918981481481481</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.69224537037037026</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.69259259259259265</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.69293981481481481</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.69328703703703709</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.69363425925925926</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.69398148148148142</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.6943287037037037</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.69467592592592586</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.69502314814814825</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.69537037037037042</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.69571759259259258</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.69606481481481486</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.69641203703703702</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.69675925925925919</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.69710648148148147</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.69745370370370363</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.69780092592592602</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.69814814814814818</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.69849537037037035</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.69884259259259263</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.69918981481481479</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Start-up Test'!#REF!</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F8FA-4640-A230-8DCCF7D0B504}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="717779032"/>
+        <c:axId val="717780672"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="717779032"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="0.70100000000000007"/>
+          <c:min val="0.68000000000000016"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Time</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="h:mm:ss" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="717780672"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="6.9444440000000019E-3"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="717780672"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="100"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Humidity (%)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="717779032"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -9762,6 +11684,86 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -10318,6 +12320,1038 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -11572,6 +14606,87 @@
 </c:userShapes>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>463550</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B121487B-3E43-448D-94F9-3CA528FE590F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>450850</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3DE270BD-DC65-4651-B8E5-FCCA558A0184}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -11871,7 +14986,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:H342"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="AI26" sqref="AI26"/>
     </sheetView>
   </sheetViews>
@@ -18684,4 +21799,1491 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E5AAC19-0A18-4477-AC69-274FDC6B5C62}">
+  <dimension ref="B3:D342"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AD42" sqref="AD42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="10.08984375" customWidth="1"/>
+    <col min="3" max="3" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B5" s="2">
+        <v>0.68078703703703702</v>
+      </c>
+      <c r="C5">
+        <v>28.869199999999999</v>
+      </c>
+      <c r="D5">
+        <v>42.961599999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B6" s="2">
+        <v>0.68113425925925919</v>
+      </c>
+      <c r="C6">
+        <v>28.5045</v>
+      </c>
+      <c r="D6">
+        <v>47.150199999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B7" s="2">
+        <v>0.68148148148148147</v>
+      </c>
+      <c r="C7">
+        <v>28.2042</v>
+      </c>
+      <c r="D7">
+        <v>51.865099999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B8" s="2">
+        <v>0.68182870370370363</v>
+      </c>
+      <c r="C8">
+        <v>28.011199999999999</v>
+      </c>
+      <c r="D8">
+        <v>55.7714</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B9" s="2">
+        <v>0.68217592592592602</v>
+      </c>
+      <c r="C9">
+        <v>27.9147</v>
+      </c>
+      <c r="D9">
+        <v>56.542000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B10" s="2">
+        <v>0.68252314814814818</v>
+      </c>
+      <c r="C10">
+        <v>27.9254</v>
+      </c>
+      <c r="D10">
+        <v>55.061900000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B11" s="2">
+        <v>0.68287037037037035</v>
+      </c>
+      <c r="C11">
+        <v>27.989699999999999</v>
+      </c>
+      <c r="D11">
+        <v>56.953899999999997</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B12" s="2">
+        <v>0.68321759259259263</v>
+      </c>
+      <c r="C12">
+        <v>28.107700000000001</v>
+      </c>
+      <c r="D12">
+        <v>60.356699999999996</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B13" s="2">
+        <v>0.68356481481481479</v>
+      </c>
+      <c r="C13">
+        <v>28.2364</v>
+      </c>
+      <c r="D13">
+        <v>60.4482</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B14" s="2">
+        <v>0.68391203703703696</v>
+      </c>
+      <c r="C14">
+        <v>28.397300000000001</v>
+      </c>
+      <c r="D14">
+        <v>62.607300000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B15" s="2">
+        <v>0.68425925925925923</v>
+      </c>
+      <c r="C15">
+        <v>28.579599999999999</v>
+      </c>
+      <c r="D15">
+        <v>62.111400000000003</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B16" s="2">
+        <v>0.68460648148148151</v>
+      </c>
+      <c r="C16">
+        <v>28.7727</v>
+      </c>
+      <c r="D16">
+        <v>62.706499999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B17" s="2">
+        <v>0.68495370370370379</v>
+      </c>
+      <c r="C17">
+        <v>28.976400000000002</v>
+      </c>
+      <c r="D17">
+        <v>63.683100000000003</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B18" s="2">
+        <v>0.68530092592592595</v>
+      </c>
+      <c r="C18">
+        <v>29.180199999999999</v>
+      </c>
+      <c r="D18">
+        <v>64.468900000000005</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B19" s="2">
+        <v>0.68564814814814812</v>
+      </c>
+      <c r="C19">
+        <v>29.3947</v>
+      </c>
+      <c r="D19">
+        <v>64.644400000000005</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B20" s="2">
+        <v>0.68599537037037039</v>
+      </c>
+      <c r="C20">
+        <v>29.598500000000001</v>
+      </c>
+      <c r="D20">
+        <v>66.048199999999994</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B21" s="2">
+        <v>0.68634259259259256</v>
+      </c>
+      <c r="C21">
+        <v>29.802299999999999</v>
+      </c>
+      <c r="D21">
+        <v>65.666700000000006</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B22" s="2">
+        <v>0.68668981481481473</v>
+      </c>
+      <c r="C22">
+        <v>30.006</v>
+      </c>
+      <c r="D22">
+        <v>66.681399999999996</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B23" s="2">
+        <v>0.687037037037037</v>
+      </c>
+      <c r="C23">
+        <v>30.209800000000001</v>
+      </c>
+      <c r="D23">
+        <v>67.375699999999995</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B24" s="2">
+        <v>0.68738425925925928</v>
+      </c>
+      <c r="C24">
+        <v>30.381399999999999</v>
+      </c>
+      <c r="D24">
+        <v>67.940299999999993</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B25" s="2">
+        <v>0.68773148148148155</v>
+      </c>
+      <c r="C25">
+        <v>30.499400000000001</v>
+      </c>
+      <c r="D25">
+        <v>68.199700000000007</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B26" s="2">
+        <v>0.68807870370370372</v>
+      </c>
+      <c r="C26">
+        <v>30.6067</v>
+      </c>
+      <c r="D26">
+        <v>68.794799999999995</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B27" s="2">
+        <v>0.68842592592592589</v>
+      </c>
+      <c r="C27">
+        <v>30.756799999999998</v>
+      </c>
+      <c r="D27">
+        <v>70.244399999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B28" s="2">
+        <v>0.68877314814814816</v>
+      </c>
+      <c r="C28">
+        <v>30.907</v>
+      </c>
+      <c r="D28">
+        <v>72.563699999999997</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B29" s="2">
+        <v>0.68912037037037033</v>
+      </c>
+      <c r="C29">
+        <v>31.046399999999998</v>
+      </c>
+      <c r="D29">
+        <v>73.67</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B30" s="2">
+        <v>0.68946759259259249</v>
+      </c>
+      <c r="C30">
+        <v>31.121500000000001</v>
+      </c>
+      <c r="D30">
+        <v>74.326099999999997</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B31" s="2">
+        <v>0.68981481481481488</v>
+      </c>
+      <c r="C31">
+        <v>31.153600000000001</v>
+      </c>
+      <c r="D31">
+        <v>74.242199999999997</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B32" s="2">
+        <v>0.69016203703703705</v>
+      </c>
+      <c r="C32">
+        <v>31.218</v>
+      </c>
+      <c r="D32">
+        <v>74.974599999999995</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B33" s="2">
+        <v>0.69050925925925932</v>
+      </c>
+      <c r="C33">
+        <v>31.314499999999999</v>
+      </c>
+      <c r="D33">
+        <v>75.806200000000004</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B34" s="2">
+        <v>0.69085648148148149</v>
+      </c>
+      <c r="C34">
+        <v>31.411000000000001</v>
+      </c>
+      <c r="D34">
+        <v>76.698800000000006</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B35" s="2">
+        <v>0.69120370370370365</v>
+      </c>
+      <c r="C35">
+        <v>31.443200000000001</v>
+      </c>
+      <c r="D35">
+        <v>77.179500000000004</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B36" s="2">
+        <v>0.69155092592592593</v>
+      </c>
+      <c r="C36">
+        <v>31.464700000000001</v>
+      </c>
+      <c r="D36">
+        <v>77.744</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B37" s="2">
+        <v>0.6918981481481481</v>
+      </c>
+      <c r="C37">
+        <v>31.529</v>
+      </c>
+      <c r="D37">
+        <v>79.979500000000002</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B38" s="2">
+        <v>0.69224537037037026</v>
+      </c>
+      <c r="C38">
+        <v>31.625499999999999</v>
+      </c>
+      <c r="D38">
+        <v>80.299899999999994</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B39" s="2">
+        <v>0.69259259259259265</v>
+      </c>
+      <c r="C39">
+        <v>31.689900000000002</v>
+      </c>
+      <c r="D39">
+        <v>81.177300000000002</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B40" s="2">
+        <v>0.69293981481481481</v>
+      </c>
+      <c r="C40">
+        <v>31.689900000000002</v>
+      </c>
+      <c r="D40">
+        <v>81.375600000000006</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B41" s="2">
+        <v>0.69328703703703709</v>
+      </c>
+      <c r="C41">
+        <v>31.689900000000002</v>
+      </c>
+      <c r="D41">
+        <v>82.092799999999997</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B42" s="2">
+        <v>0.69363425925925926</v>
+      </c>
+      <c r="C42">
+        <v>31.722100000000001</v>
+      </c>
+      <c r="D42">
+        <v>82.672600000000003</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B43" s="2">
+        <v>0.69398148148148142</v>
+      </c>
+      <c r="C43">
+        <v>31.7971</v>
+      </c>
+      <c r="D43">
+        <v>84.602900000000005</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B44" s="2">
+        <v>0.6943287037037037</v>
+      </c>
+      <c r="C44">
+        <v>31.861499999999999</v>
+      </c>
+      <c r="D44">
+        <v>84.602900000000005</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B45" s="2">
+        <v>0.69467592592592586</v>
+      </c>
+      <c r="C45">
+        <v>31.872199999999999</v>
+      </c>
+      <c r="D45">
+        <v>85.152199999999993</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B46" s="2">
+        <v>0.69502314814814825</v>
+      </c>
+      <c r="C46">
+        <v>31.84</v>
+      </c>
+      <c r="D46">
+        <v>85.793099999999995</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B47" s="2">
+        <v>0.69537037037037042</v>
+      </c>
+      <c r="C47">
+        <v>31.84</v>
+      </c>
+      <c r="D47">
+        <v>86.8917</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B48" s="2">
+        <v>0.69571759259259258</v>
+      </c>
+      <c r="C48">
+        <v>31.904399999999999</v>
+      </c>
+      <c r="D48">
+        <v>87.593599999999995</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B49" s="2">
+        <v>0.69606481481481486</v>
+      </c>
+      <c r="C49">
+        <v>31.925799999999999</v>
+      </c>
+      <c r="D49">
+        <v>87.998000000000005</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B50" s="2">
+        <v>0.69641203703703702</v>
+      </c>
+      <c r="C50">
+        <v>31.936599999999999</v>
+      </c>
+      <c r="D50">
+        <v>88.173400000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B51" s="2">
+        <v>0.69675925925925919</v>
+      </c>
+      <c r="C51">
+        <v>31.925799999999999</v>
+      </c>
+      <c r="D51">
+        <v>88.257400000000004</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B52" s="2">
+        <v>0.69710648148148147</v>
+      </c>
+      <c r="C52">
+        <v>31.925799999999999</v>
+      </c>
+      <c r="D52">
+        <v>88.898200000000003</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B53" s="2">
+        <v>0.69745370370370363</v>
+      </c>
+      <c r="C53">
+        <v>31.936599999999999</v>
+      </c>
+      <c r="D53">
+        <v>89.554400000000001</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B54" s="2">
+        <v>0.69780092592592602</v>
+      </c>
+      <c r="C54">
+        <v>31.936599999999999</v>
+      </c>
+      <c r="D54">
+        <v>89.874799999999993</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B55" s="2">
+        <v>0.69814814814814818</v>
+      </c>
+      <c r="C55">
+        <v>31.936599999999999</v>
+      </c>
+      <c r="D55">
+        <v>89.523799999999994</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B56" s="2">
+        <v>0.69849537037037035</v>
+      </c>
+      <c r="C56">
+        <v>31.936599999999999</v>
+      </c>
+      <c r="D56">
+        <v>89.813800000000001</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B57" s="2">
+        <v>0.69884259259259263</v>
+      </c>
+      <c r="C57">
+        <v>31.957999999999998</v>
+      </c>
+      <c r="D57">
+        <v>90.080799999999996</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B58" s="2">
+        <v>0.69918981481481479</v>
+      </c>
+      <c r="C58">
+        <v>32.000900000000001</v>
+      </c>
+      <c r="D58">
+        <v>90.485100000000003</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B59" s="2"/>
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B60" s="2"/>
+    </row>
+    <row r="61" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B61" s="2"/>
+    </row>
+    <row r="62" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B62" s="2"/>
+    </row>
+    <row r="63" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B63" s="2"/>
+    </row>
+    <row r="64" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B64" s="2"/>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B65" s="2"/>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B66" s="2"/>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B67" s="2"/>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B68" s="2"/>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B69" s="2"/>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B70" s="2"/>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B71" s="2"/>
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B72" s="2"/>
+    </row>
+    <row r="73" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B73" s="2"/>
+    </row>
+    <row r="74" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B74" s="2"/>
+    </row>
+    <row r="75" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B75" s="2"/>
+    </row>
+    <row r="76" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B76" s="2"/>
+    </row>
+    <row r="77" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B77" s="2"/>
+    </row>
+    <row r="78" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B78" s="2"/>
+    </row>
+    <row r="79" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B79" s="2"/>
+    </row>
+    <row r="80" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B80" s="2"/>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B81" s="2"/>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B82" s="2"/>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B83" s="2"/>
+    </row>
+    <row r="84" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B84" s="2"/>
+    </row>
+    <row r="85" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B85" s="2"/>
+    </row>
+    <row r="86" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B86" s="2"/>
+    </row>
+    <row r="87" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B87" s="2"/>
+    </row>
+    <row r="88" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B88" s="2"/>
+    </row>
+    <row r="89" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B89" s="2"/>
+    </row>
+    <row r="90" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B90" s="2"/>
+    </row>
+    <row r="91" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B91" s="2"/>
+    </row>
+    <row r="92" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B92" s="2"/>
+    </row>
+    <row r="93" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B93" s="2"/>
+    </row>
+    <row r="94" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B94" s="2"/>
+    </row>
+    <row r="95" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B95" s="2"/>
+    </row>
+    <row r="96" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B96" s="2"/>
+    </row>
+    <row r="97" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B97" s="2"/>
+    </row>
+    <row r="98" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B98" s="2"/>
+    </row>
+    <row r="99" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B99" s="2"/>
+    </row>
+    <row r="100" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B100" s="2"/>
+    </row>
+    <row r="101" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B101" s="2"/>
+    </row>
+    <row r="102" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B102" s="2"/>
+    </row>
+    <row r="103" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B103" s="2"/>
+    </row>
+    <row r="104" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B104" s="2"/>
+    </row>
+    <row r="105" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B105" s="2"/>
+    </row>
+    <row r="106" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B106" s="2"/>
+    </row>
+    <row r="107" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B107" s="2"/>
+    </row>
+    <row r="108" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B108" s="2"/>
+    </row>
+    <row r="109" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B109" s="2"/>
+    </row>
+    <row r="110" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B110" s="2"/>
+    </row>
+    <row r="111" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B111" s="2"/>
+    </row>
+    <row r="112" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B112" s="2"/>
+    </row>
+    <row r="113" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B113" s="2"/>
+    </row>
+    <row r="114" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B114" s="2"/>
+    </row>
+    <row r="115" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B115" s="2"/>
+    </row>
+    <row r="116" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B116" s="2"/>
+    </row>
+    <row r="117" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B117" s="2"/>
+    </row>
+    <row r="118" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B118" s="2"/>
+    </row>
+    <row r="119" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B119" s="2"/>
+    </row>
+    <row r="120" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B120" s="2"/>
+    </row>
+    <row r="121" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B121" s="2"/>
+    </row>
+    <row r="122" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B122" s="2"/>
+    </row>
+    <row r="123" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B123" s="2"/>
+    </row>
+    <row r="124" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B124" s="2"/>
+    </row>
+    <row r="125" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B125" s="2"/>
+    </row>
+    <row r="126" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B126" s="2"/>
+    </row>
+    <row r="127" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B127" s="2"/>
+    </row>
+    <row r="128" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B128" s="2"/>
+    </row>
+    <row r="129" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B129" s="2"/>
+    </row>
+    <row r="130" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B130" s="2"/>
+    </row>
+    <row r="131" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B131" s="2"/>
+    </row>
+    <row r="132" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B132" s="2"/>
+    </row>
+    <row r="133" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B133" s="2"/>
+    </row>
+    <row r="134" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B134" s="2"/>
+    </row>
+    <row r="135" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B135" s="2"/>
+    </row>
+    <row r="136" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B136" s="2"/>
+    </row>
+    <row r="137" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B137" s="2"/>
+    </row>
+    <row r="138" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B138" s="2"/>
+    </row>
+    <row r="139" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B139" s="2"/>
+    </row>
+    <row r="140" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B140" s="2"/>
+    </row>
+    <row r="141" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B141" s="2"/>
+    </row>
+    <row r="142" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B142" s="2"/>
+    </row>
+    <row r="143" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B143" s="2"/>
+    </row>
+    <row r="144" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B144" s="2"/>
+    </row>
+    <row r="145" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B145" s="2"/>
+    </row>
+    <row r="146" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B146" s="2"/>
+    </row>
+    <row r="147" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B147" s="2"/>
+    </row>
+    <row r="148" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B148" s="2"/>
+    </row>
+    <row r="149" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B149" s="2"/>
+    </row>
+    <row r="150" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B150" s="2"/>
+    </row>
+    <row r="151" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B151" s="2"/>
+    </row>
+    <row r="152" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B152" s="2"/>
+    </row>
+    <row r="153" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B153" s="2"/>
+    </row>
+    <row r="154" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B154" s="2"/>
+    </row>
+    <row r="155" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B155" s="2"/>
+    </row>
+    <row r="156" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B156" s="2"/>
+    </row>
+    <row r="157" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B157" s="2"/>
+    </row>
+    <row r="158" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B158" s="2"/>
+    </row>
+    <row r="159" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B159" s="2"/>
+    </row>
+    <row r="160" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B160" s="2"/>
+    </row>
+    <row r="161" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B161" s="2"/>
+    </row>
+    <row r="162" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B162" s="2"/>
+    </row>
+    <row r="163" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B163" s="2"/>
+    </row>
+    <row r="164" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B164" s="2"/>
+    </row>
+    <row r="165" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B165" s="2"/>
+    </row>
+    <row r="166" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B166" s="2"/>
+    </row>
+    <row r="167" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B167" s="2"/>
+    </row>
+    <row r="168" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B168" s="2"/>
+    </row>
+    <row r="169" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B169" s="2"/>
+    </row>
+    <row r="170" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B170" s="2"/>
+    </row>
+    <row r="171" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B171" s="2"/>
+    </row>
+    <row r="172" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B172" s="2"/>
+    </row>
+    <row r="173" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B173" s="2"/>
+    </row>
+    <row r="174" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B174" s="2"/>
+    </row>
+    <row r="175" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B175" s="2"/>
+    </row>
+    <row r="176" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B176" s="2"/>
+    </row>
+    <row r="177" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B177" s="2"/>
+    </row>
+    <row r="178" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B178" s="2"/>
+    </row>
+    <row r="179" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B179" s="2"/>
+    </row>
+    <row r="180" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B180" s="2"/>
+    </row>
+    <row r="181" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B181" s="2"/>
+    </row>
+    <row r="182" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B182" s="2"/>
+    </row>
+    <row r="183" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B183" s="2"/>
+    </row>
+    <row r="184" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B184" s="2"/>
+    </row>
+    <row r="185" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B185" s="2"/>
+    </row>
+    <row r="186" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B186" s="2"/>
+    </row>
+    <row r="187" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B187" s="2"/>
+    </row>
+    <row r="188" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B188" s="2"/>
+    </row>
+    <row r="189" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B189" s="2"/>
+    </row>
+    <row r="190" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B190" s="2"/>
+    </row>
+    <row r="191" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B191" s="2"/>
+    </row>
+    <row r="192" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B192" s="2"/>
+    </row>
+    <row r="193" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B193" s="2"/>
+    </row>
+    <row r="194" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B194" s="2"/>
+    </row>
+    <row r="195" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B195" s="2"/>
+    </row>
+    <row r="196" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B196" s="2"/>
+    </row>
+    <row r="197" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B197" s="2"/>
+    </row>
+    <row r="198" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B198" s="2"/>
+    </row>
+    <row r="199" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B199" s="2"/>
+    </row>
+    <row r="200" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B200" s="2"/>
+    </row>
+    <row r="201" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B201" s="2"/>
+    </row>
+    <row r="202" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B202" s="2"/>
+    </row>
+    <row r="203" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B203" s="2"/>
+    </row>
+    <row r="204" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B204" s="2"/>
+    </row>
+    <row r="205" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B205" s="2"/>
+    </row>
+    <row r="206" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B206" s="2"/>
+    </row>
+    <row r="207" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B207" s="2"/>
+    </row>
+    <row r="208" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B208" s="2"/>
+    </row>
+    <row r="209" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B209" s="2"/>
+    </row>
+    <row r="210" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B210" s="2"/>
+    </row>
+    <row r="211" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B211" s="2"/>
+    </row>
+    <row r="212" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B212" s="2"/>
+    </row>
+    <row r="213" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B213" s="2"/>
+    </row>
+    <row r="214" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B214" s="2"/>
+    </row>
+    <row r="215" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B215" s="2"/>
+    </row>
+    <row r="216" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B216" s="2"/>
+    </row>
+    <row r="217" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B217" s="2"/>
+    </row>
+    <row r="218" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B218" s="2"/>
+    </row>
+    <row r="219" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B219" s="2"/>
+    </row>
+    <row r="220" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B220" s="2"/>
+    </row>
+    <row r="221" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B221" s="2"/>
+    </row>
+    <row r="222" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B222" s="2"/>
+    </row>
+    <row r="223" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B223" s="2"/>
+    </row>
+    <row r="224" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B224" s="2"/>
+    </row>
+    <row r="225" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B225" s="2"/>
+    </row>
+    <row r="226" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B226" s="2"/>
+    </row>
+    <row r="227" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B227" s="2"/>
+    </row>
+    <row r="228" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B228" s="2"/>
+    </row>
+    <row r="229" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B229" s="2"/>
+    </row>
+    <row r="230" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B230" s="2"/>
+    </row>
+    <row r="231" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B231" s="2"/>
+    </row>
+    <row r="232" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B232" s="2"/>
+    </row>
+    <row r="233" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B233" s="2"/>
+    </row>
+    <row r="234" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B234" s="2"/>
+    </row>
+    <row r="235" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B235" s="2"/>
+    </row>
+    <row r="236" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B236" s="2"/>
+    </row>
+    <row r="237" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B237" s="2"/>
+    </row>
+    <row r="238" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B238" s="2"/>
+    </row>
+    <row r="239" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B239" s="2"/>
+    </row>
+    <row r="240" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B240" s="2"/>
+    </row>
+    <row r="241" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B241" s="2"/>
+    </row>
+    <row r="242" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B242" s="2"/>
+    </row>
+    <row r="243" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B243" s="2"/>
+    </row>
+    <row r="244" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B244" s="2"/>
+    </row>
+    <row r="245" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B245" s="2"/>
+    </row>
+    <row r="246" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B246" s="2"/>
+    </row>
+    <row r="247" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B247" s="2"/>
+    </row>
+    <row r="248" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B248" s="2"/>
+    </row>
+    <row r="249" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B249" s="2"/>
+    </row>
+    <row r="250" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B250" s="2"/>
+    </row>
+    <row r="251" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B251" s="2"/>
+    </row>
+    <row r="252" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B252" s="2"/>
+    </row>
+    <row r="253" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B253" s="2"/>
+    </row>
+    <row r="254" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B254" s="2"/>
+    </row>
+    <row r="255" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B255" s="2"/>
+    </row>
+    <row r="256" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B256" s="2"/>
+    </row>
+    <row r="257" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B257" s="2"/>
+    </row>
+    <row r="258" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B258" s="2"/>
+    </row>
+    <row r="259" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B259" s="2"/>
+    </row>
+    <row r="260" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B260" s="2"/>
+    </row>
+    <row r="261" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B261" s="2"/>
+    </row>
+    <row r="262" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B262" s="2"/>
+    </row>
+    <row r="263" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B263" s="2"/>
+    </row>
+    <row r="264" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B264" s="2"/>
+    </row>
+    <row r="265" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B265" s="2"/>
+    </row>
+    <row r="266" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B266" s="2"/>
+    </row>
+    <row r="267" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B267" s="2"/>
+    </row>
+    <row r="268" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B268" s="2"/>
+    </row>
+    <row r="269" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B269" s="2"/>
+    </row>
+    <row r="270" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B270" s="2"/>
+    </row>
+    <row r="271" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B271" s="2"/>
+    </row>
+    <row r="272" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B272" s="2"/>
+    </row>
+    <row r="273" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B273" s="2"/>
+    </row>
+    <row r="274" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B274" s="2"/>
+    </row>
+    <row r="275" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B275" s="2"/>
+    </row>
+    <row r="276" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B276" s="2"/>
+    </row>
+    <row r="277" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B277" s="2"/>
+    </row>
+    <row r="278" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B278" s="2"/>
+    </row>
+    <row r="279" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B279" s="2"/>
+    </row>
+    <row r="280" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B280" s="2"/>
+    </row>
+    <row r="281" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B281" s="2"/>
+    </row>
+    <row r="282" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B282" s="2"/>
+    </row>
+    <row r="283" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B283" s="2"/>
+    </row>
+    <row r="284" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B284" s="2"/>
+    </row>
+    <row r="285" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B285" s="2"/>
+    </row>
+    <row r="286" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B286" s="2"/>
+    </row>
+    <row r="287" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B287" s="2"/>
+    </row>
+    <row r="288" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B288" s="2"/>
+    </row>
+    <row r="289" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B289" s="2"/>
+    </row>
+    <row r="290" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B290" s="2"/>
+    </row>
+    <row r="291" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B291" s="2"/>
+    </row>
+    <row r="292" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B292" s="2"/>
+    </row>
+    <row r="293" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B293" s="2"/>
+    </row>
+    <row r="294" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B294" s="2"/>
+    </row>
+    <row r="295" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B295" s="2"/>
+    </row>
+    <row r="296" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B296" s="2"/>
+    </row>
+    <row r="297" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B297" s="2"/>
+    </row>
+    <row r="298" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B298" s="2"/>
+    </row>
+    <row r="299" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B299" s="2"/>
+    </row>
+    <row r="300" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B300" s="2"/>
+    </row>
+    <row r="301" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B301" s="2"/>
+    </row>
+    <row r="302" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B302" s="2"/>
+    </row>
+    <row r="303" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B303" s="2"/>
+    </row>
+    <row r="304" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B304" s="2"/>
+    </row>
+    <row r="305" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B305" s="2"/>
+    </row>
+    <row r="306" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B306" s="2"/>
+    </row>
+    <row r="307" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B307" s="2"/>
+    </row>
+    <row r="308" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B308" s="2"/>
+    </row>
+    <row r="309" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B309" s="2"/>
+    </row>
+    <row r="310" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B310" s="2"/>
+    </row>
+    <row r="311" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B311" s="2"/>
+    </row>
+    <row r="312" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B312" s="2"/>
+    </row>
+    <row r="313" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B313" s="2"/>
+    </row>
+    <row r="314" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B314" s="2"/>
+    </row>
+    <row r="315" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B315" s="2"/>
+    </row>
+    <row r="316" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B316" s="2"/>
+    </row>
+    <row r="317" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B317" s="2"/>
+    </row>
+    <row r="318" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B318" s="2"/>
+    </row>
+    <row r="319" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B319" s="2"/>
+    </row>
+    <row r="320" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B320" s="2"/>
+    </row>
+    <row r="321" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B321" s="2"/>
+    </row>
+    <row r="322" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B322" s="2"/>
+    </row>
+    <row r="323" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B323" s="2"/>
+    </row>
+    <row r="324" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B324" s="2"/>
+    </row>
+    <row r="325" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B325" s="2"/>
+    </row>
+    <row r="326" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B326" s="2"/>
+    </row>
+    <row r="327" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B327" s="2"/>
+    </row>
+    <row r="328" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B328" s="2"/>
+    </row>
+    <row r="329" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B329" s="2"/>
+    </row>
+    <row r="330" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B330" s="2"/>
+    </row>
+    <row r="331" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B331" s="2"/>
+    </row>
+    <row r="332" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B332" s="2"/>
+    </row>
+    <row r="333" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B333" s="2"/>
+    </row>
+    <row r="334" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B334" s="2"/>
+    </row>
+    <row r="335" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B335" s="2"/>
+    </row>
+    <row r="336" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B336" s="2"/>
+    </row>
+    <row r="337" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B337" s="2"/>
+    </row>
+    <row r="338" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B338" s="2"/>
+    </row>
+    <row r="339" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B339" s="2"/>
+    </row>
+    <row r="340" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B340" s="2"/>
+    </row>
+    <row r="341" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B341" s="2"/>
+    </row>
+    <row r="342" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B342" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C3:D3"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>